<commit_message>
- Change value box color - Add delay command in arduino - Manage database - Add equipment datasheet
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe\PE\ext_Resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAADCD-8738-482C-833F-BD40FAF20ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE1965C-1E5F-47C0-B0B7-4EC8570B3734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="BMW" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t>Contact Pairs</t>
   </si>
@@ -100,18 +100,9 @@
     <t>MPAC1 to MPEC1</t>
   </si>
   <si>
-    <t>OBC</t>
-  </si>
-  <si>
     <t>DCB1.2H</t>
   </si>
   <si>
-    <t>DCB2.0</t>
-  </si>
-  <si>
-    <t>5DH</t>
-  </si>
-  <si>
     <t>NISSAN</t>
   </si>
   <si>
@@ -122,6 +113,138 @@
   </si>
   <si>
     <t>Setpoint Current</t>
+  </si>
+  <si>
+    <t>MP1 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP2 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP3 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP4 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP1 to MPEC2</t>
+  </si>
+  <si>
+    <t>MP2 to MPEC2</t>
+  </si>
+  <si>
+    <t>MP3 to MPEC2</t>
+  </si>
+  <si>
+    <t>MP1 to MPEC3</t>
+  </si>
+  <si>
+    <t>MP2 to MPEC3</t>
+  </si>
+  <si>
+    <t>MP3 to MPEC3</t>
+  </si>
+  <si>
+    <t>MP1 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP2 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP3 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP1 to MPEC2 (RE)</t>
+  </si>
+  <si>
+    <t>MP2 to MPEC2 (RE)</t>
+  </si>
+  <si>
+    <t>MP3 to MPEC2 (RE)</t>
+  </si>
+  <si>
+    <t>MP1 to MPEC3 (RE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MP2 to MPEC3 (RE)</t>
+  </si>
+  <si>
+    <t>MP3 to MPEC3 (RE)</t>
+  </si>
+  <si>
+    <t>MP5 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP6 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP7 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP8 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP9 to MPE (RE)</t>
+  </si>
+  <si>
+    <t>MP4 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MP5 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP6 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP7 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP8 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MP9 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MPAC1 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>MPAC2 to MPEC1 (RE)</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPEC</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPEC</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPE</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPE</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPEC (RE)</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPEC (RE)</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPE (RE)</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPE (RE)</t>
+  </si>
+  <si>
+    <t>Cover center to Chassis GND</t>
+  </si>
+  <si>
+    <t>Cover Edge to Chassis GND</t>
+  </si>
+  <si>
+    <t>Cover center to Chassis GND (RE)</t>
+  </si>
+  <si>
+    <t>Cover Edge to Chassis GND (RE)</t>
   </si>
 </sst>
 </file>
@@ -158,10 +281,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,17 +606,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -497,11 +628,11 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -511,10 +642,10 @@
       <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>25</v>
       </c>
     </row>
@@ -542,24 +673,58 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B3C947-D757-45AA-817A-4B43C428C667}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -569,26 +734,236 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -597,17 +972,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4A438-F966-48A2-AFD5-D9139D663046}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -617,11 +994,11 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -631,10 +1008,10 @@
       <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>25</v>
       </c>
     </row>
@@ -787,6 +1164,166 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="1">
         <v>20</v>
       </c>
     </row>
@@ -800,12 +1337,165 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -817,113 +1507,56 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -935,14 +1568,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -952,21 +1587,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>25</v>
       </c>
     </row>
@@ -979,15 +1614,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -997,25 +1634,29 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Make database file look colorful
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe\PE\ext_Resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE1965C-1E5F-47C0-B0B7-4EC8570B3734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B18D3F-E087-4FFD-84F9-5BB837976B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
@@ -261,12 +261,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -281,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,6 +314,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,86 +661,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>10</v>
       </c>
     </row>
@@ -715,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B3C947-D757-45AA-817A-4B43C428C667}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,238 +767,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="5">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>20</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>20</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>20</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>20</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>20</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>20</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>20</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>20</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>10</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>20</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="5">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>20</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="5">
         <v>20</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>20</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <v>20</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <v>20</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <v>20</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <v>20</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <v>10</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <v>10</v>
       </c>
       <c r="C23" s="2"/>
@@ -974,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4A438-F966-48A2-AFD5-D9139D663046}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,342 +1027,342 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="5">
         <v>20</v>
       </c>
     </row>
@@ -1336,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C5E0E7-8060-4401-A9FF-74A0D7403DC3}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,27 +1389,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
@@ -1383,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1397,86 +1439,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1489,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1501,58 +1543,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="3">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="8">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6">
         <v>0.02</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="8">
         <v>20</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="8">
         <v>20</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="8">
         <v>20</v>
       </c>
       <c r="C5" s="3"/>
@@ -1567,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A96459A-EFE5-49DC-B9F0-72C636BBE5E1}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1581,27 +1623,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>
@@ -1614,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1628,30 +1673,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add help >>> Spec (BMW,OBC,DCB,5DH,NISSAN) information dialog
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe\PE\ext_Resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B18D3F-E087-4FFD-84F9-5BB837976B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAAFB6A-E4EA-489C-B005-A34A087AD9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="BMW" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Contact Pairs</t>
   </si>
@@ -103,9 +103,6 @@
     <t>DCB1.2H</t>
   </si>
   <si>
-    <t>NISSAN</t>
-  </si>
-  <si>
     <t>CUSTOM</t>
   </si>
   <si>
@@ -245,6 +242,15 @@
   </si>
   <si>
     <t>Cover Edge to Chassis GND (RE)</t>
+  </si>
+  <si>
+    <t>MPE to MP1</t>
+  </si>
+  <si>
+    <t>MPE to MP2</t>
+  </si>
+  <si>
+    <t>MPR to MP3</t>
   </si>
 </sst>
 </file>
@@ -647,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,10 +674,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -714,7 +720,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
         <v>10</v>
@@ -722,7 +728,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="5">
         <v>10</v>
@@ -730,7 +736,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -738,7 +744,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
@@ -755,7 +761,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F28" sqref="A1:XFD1048576"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -774,10 +780,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -816,7 +822,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5">
         <v>20</v>
@@ -826,7 +832,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5">
         <v>20</v>
@@ -836,7 +842,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5">
         <v>20</v>
@@ -846,7 +852,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="5">
         <v>20</v>
@@ -856,7 +862,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5">
         <v>20</v>
@@ -866,7 +872,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5">
         <v>20</v>
@@ -896,7 +902,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5">
         <v>20</v>
@@ -906,7 +912,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5">
         <v>20</v>
@@ -916,7 +922,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5">
         <v>20</v>
@@ -926,7 +932,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="5">
         <v>20</v>
@@ -936,7 +942,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5">
         <v>20</v>
@@ -946,7 +952,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="5">
         <v>20</v>
@@ -956,7 +962,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="5">
         <v>20</v>
@@ -966,7 +972,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="5">
         <v>20</v>
@@ -976,7 +982,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="5">
         <v>20</v>
@@ -986,7 +992,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5">
         <v>10</v>
@@ -996,7 +1002,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="5">
         <v>10</v>
@@ -1014,7 +1020,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D41"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1034,10 +1040,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1208,7 +1214,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5">
         <v>10</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="5">
         <v>10</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5">
         <v>10</v>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="5">
         <v>10</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5">
         <v>10</v>
@@ -1248,7 +1254,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="5">
         <v>10</v>
@@ -1256,7 +1262,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5">
         <v>10</v>
@@ -1264,7 +1270,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="5">
         <v>10</v>
@@ -1272,7 +1278,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="5">
         <v>10</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="5">
         <v>20</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="5">
         <v>20</v>
@@ -1296,7 +1302,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="5">
         <v>20</v>
@@ -1304,7 +1310,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="5">
         <v>20</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="5">
         <v>20</v>
@@ -1320,7 +1326,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5">
         <v>20</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="5">
         <v>20</v>
@@ -1336,7 +1342,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" s="5">
         <v>20</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="5">
         <v>20</v>
@@ -1352,7 +1358,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="5">
         <v>20</v>
@@ -1360,7 +1366,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" s="5">
         <v>20</v>
@@ -1376,7 +1382,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1396,10 +1402,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1426,7 +1432,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1446,15 +1452,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5">
         <v>20</v>
@@ -1468,7 +1474,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="5">
         <v>20</v>
@@ -1476,7 +1482,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5">
         <v>10</v>
@@ -1484,7 +1490,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5">
         <v>10</v>
@@ -1492,7 +1498,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="5">
         <v>20</v>
@@ -1500,7 +1506,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="5">
         <v>20</v>
@@ -1508,7 +1514,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -1516,7 +1522,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
@@ -1532,7 +1538,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1550,15 +1556,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="8">
         <v>20</v>
@@ -1572,7 +1578,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="8">
         <v>20</v>
@@ -1582,7 +1588,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="8">
         <v>20</v>
@@ -1592,7 +1598,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="8">
         <v>20</v>
@@ -1607,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A96459A-EFE5-49DC-B9F0-72C636BBE5E1}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1630,15 +1636,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B2" s="5">
         <v>10</v>
@@ -1648,6 +1654,22 @@
       </c>
       <c r="D2" s="7">
         <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1682,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="A1:XFD1048576"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1680,15 +1702,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5">
         <v>10</v>

</xml_diff>

<commit_message>
Add help >>> spec >>> each project spec
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe\PE\ext_Resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAAFB6A-E4EA-489C-B005-A34A087AD9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCCE646-0E55-428D-AE58-5411A0E915AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="BMW" sheetId="3" r:id="rId1"/>
@@ -232,18 +232,6 @@
     <t>DCB_BC to MPE (RE)</t>
   </si>
   <si>
-    <t>Cover center to Chassis GND</t>
-  </si>
-  <si>
-    <t>Cover Edge to Chassis GND</t>
-  </si>
-  <si>
-    <t>Cover center to Chassis GND (RE)</t>
-  </si>
-  <si>
-    <t>Cover Edge to Chassis GND (RE)</t>
-  </si>
-  <si>
     <t>MPE to MP1</t>
   </si>
   <si>
@@ -251,6 +239,18 @@
   </si>
   <si>
     <t>MPR to MP3</t>
+  </si>
+  <si>
+    <t>GND (P1) to Cover Center (P2)</t>
+  </si>
+  <si>
+    <t>GND (P1) to Cover Center (P2) (RE)</t>
+  </si>
+  <si>
+    <t>GND (P1) to Cover Edge (P2)</t>
+  </si>
+  <si>
+    <t>GND (P1) to Cover Edge (P2) (RE)</t>
   </si>
 </sst>
 </file>
@@ -1537,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B2" s="8">
         <v>20</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B3" s="8">
         <v>20</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="8">
         <v>20</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B5" s="8">
         <v>20</v>
@@ -1615,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A96459A-EFE5-49DC-B9F0-72C636BBE5E1}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5">
         <v>10</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>

</xml_diff>

<commit_message>
Remove OBC PE Chassis
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe\PE\ext_Resources\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCCE646-0E55-428D-AE58-5411A0E915AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921D75D-1CA5-43CB-97A2-29C26B45A9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="BMW" sheetId="3" r:id="rId1"/>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4A438-F966-48A2-AFD5-D9139D663046}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -1537,7 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 7.4kW CCU L v1.10.4
- Add 7.4kW CCU L
- Add 7.4kW CCU S
- Change BMW CCU list to 22kW CCU L
- Add database
</commit_message>
<xml_diff>
--- a/PE/ext_Resources/file/pe_database.xlsx
+++ b/PE/ext_Resources/file/pe_database.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe-PE\PE\ext_Resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921D75D-1CA5-43CB-97A2-29C26B45A9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6021FFF-931B-477B-ACF7-20C0A55B214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
-    <sheet name="BMW" sheetId="3" r:id="rId1"/>
-    <sheet name="DAI_OBC" sheetId="4" r:id="rId2"/>
-    <sheet name="DAI_DCB1.2" sheetId="1" r:id="rId3"/>
-    <sheet name="DAI_DCB1.2H" sheetId="5" r:id="rId4"/>
-    <sheet name="DAI_DCB2.0" sheetId="6" r:id="rId5"/>
-    <sheet name="REN_5DH" sheetId="7" r:id="rId6"/>
-    <sheet name="NISSAN_OBC" sheetId="8" r:id="rId7"/>
-    <sheet name="CUSTOM" sheetId="9" r:id="rId8"/>
+    <sheet name="7.4kW_CCU_L" sheetId="11" r:id="rId1"/>
+    <sheet name="7.4kW_CCU_S" sheetId="10" r:id="rId2"/>
+    <sheet name="22kW_CCU_L" sheetId="3" r:id="rId3"/>
+    <sheet name="DAI_OBC" sheetId="4" r:id="rId4"/>
+    <sheet name="DAI_DCB1.2" sheetId="1" r:id="rId5"/>
+    <sheet name="DAI_DCB1.2H" sheetId="5" r:id="rId6"/>
+    <sheet name="DAI_DCB2.0" sheetId="6" r:id="rId7"/>
+    <sheet name="REN_5DH" sheetId="7" r:id="rId8"/>
+    <sheet name="NISSAN_OBC" sheetId="8" r:id="rId9"/>
+    <sheet name="CUSTOM" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t>Contact Pairs</t>
   </si>
@@ -256,12 +258,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -342,7 +344,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{4C909737-61F7-4F49-A89A-6D335BD6DD85}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,23 +654,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C833A5FB-9A69-44F9-A380-760933D3676C}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -680,7 +684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -694,7 +698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -702,7 +706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -710,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -718,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -726,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -734,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -742,12 +746,63 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -757,6 +812,220 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1F2C6A-CE59-487B-BA95-DCC95811EF13}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B3C947-D757-45AA-817A-4B43C428C667}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -764,15 +1033,15 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -786,7 +1055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -800,7 +1069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -810,7 +1079,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -820,7 +1089,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -830,7 +1099,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
@@ -840,7 +1109,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
@@ -850,7 +1119,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -860,7 +1129,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -870,7 +1139,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -880,7 +1149,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -890,7 +1159,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -900,7 +1169,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -910,7 +1179,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -920,7 +1189,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -930,7 +1199,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
@@ -940,7 +1209,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
@@ -950,7 +1219,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -960,7 +1229,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -970,7 +1239,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>43</v>
       </c>
@@ -980,7 +1249,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -990,7 +1259,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1000,7 +1269,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
@@ -1015,24 +1284,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4A438-F966-48A2-AFD5-D9139D663046}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1060,7 +1329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1084,7 +1353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1092,7 +1361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1116,7 +1385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1124,7 +1393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1401,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1140,7 +1409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1172,7 +1441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1188,7 +1457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1196,7 +1465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1212,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1220,7 +1489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -1228,7 +1497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -1244,7 +1513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>45</v>
       </c>
@@ -1252,7 +1521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>46</v>
       </c>
@@ -1260,7 +1529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
@@ -1268,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>48</v>
       </c>
@@ -1276,7 +1545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>49</v>
       </c>
@@ -1284,7 +1553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
@@ -1292,7 +1561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
@@ -1300,7 +1569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
@@ -1316,7 +1585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>51</v>
       </c>
@@ -1324,7 +1593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>52</v>
       </c>
@@ -1332,7 +1601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>53</v>
       </c>
@@ -1340,7 +1609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>54</v>
       </c>
@@ -1348,7 +1617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>55</v>
       </c>
@@ -1356,7 +1625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>56</v>
       </c>
@@ -1364,7 +1633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>57</v>
       </c>
@@ -1377,7 +1646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C5E0E7-8060-4401-A9FF-74A0D7403DC3}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1385,16 +1654,16 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1427,7 +1696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1435,16 +1704,16 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
@@ -1472,7 +1741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -1480,7 +1749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -1488,7 +1757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -1496,7 +1765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
@@ -1504,7 +1773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -1512,7 +1781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -1520,7 +1789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>65</v>
       </c>
@@ -1533,7 +1802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1541,14 +1810,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1576,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
@@ -1586,7 +1855,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>70</v>
       </c>
@@ -1596,7 +1865,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>72</v>
       </c>
@@ -1611,7 +1880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A96459A-EFE5-49DC-B9F0-72C636BBE5E1}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1619,16 +1888,16 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -1656,7 +1925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1664,7 +1933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -1675,55 +1944,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="5">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>